<commit_message>
actualización proyectos en consulta Alianza pacifico
</commit_message>
<xml_diff>
--- a/docs_en_act_reg_cons_pub.xlsx
+++ b/docs_en_act_reg_cons_pub.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MarceloThompson\Documents\Programación\portal-ilar-v3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AB3D828-CBE1-4AFE-93BE-ABFACF900113}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A83D807-454D-4115-B798-8A30A7CE690F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{32A1571C-4D20-4BEB-A921-4779E9CF2709}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>PAÍS</t>
   </si>
@@ -110,6 +110,9 @@
   </si>
   <si>
     <t>Alianza del Pacífico</t>
+  </si>
+  <si>
+    <t>https://alianzapacifico.net/download/decision-no-9-anexo-suplementos-alimenticios-eliminacion-de-obstaculos-tecnicos/</t>
   </si>
 </sst>
 </file>
@@ -549,8 +552,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{348E7823-E54A-4C58-A1F2-3A90F1A67E32}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -656,12 +659,16 @@
       <c r="D6" s="5">
         <v>43831</v>
       </c>
+      <c r="E6" s="6" t="s">
+        <v>23</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" xr:uid="{7A449427-FD11-4608-A106-CFD48DD6F565}"/>
     <hyperlink ref="E3" r:id="rId2" xr:uid="{6FEA970F-8880-4A4D-AF9A-9693786797C3}"/>
     <hyperlink ref="E5" r:id="rId3" xr:uid="{B683E5B1-459E-432F-B729-CD93A345F659}"/>
+    <hyperlink ref="E6" r:id="rId4" xr:uid="{B7AC4410-2F71-4EC4-9B74-46C64AB06DDF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>